<commit_message>
Modified GanttChart, Added Formatting to the Menu, I have a bug with options Menu so expect that in the next commit
</commit_message>
<xml_diff>
--- a/doc/JAGanttChart.xlsx
+++ b/doc/JAGanttChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Programming\Team4Game\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586A48E8-6766-4D51-B982-0FCE884A69A5}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C44040-4E80-4AD3-8DDA-9B3CD30F7CD3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="4440" xr2:uid="{6FA9B399-C385-4C01-A8E4-A4B4B0C49CEF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>1 Software Analysis</t>
   </si>
@@ -46,6 +46,18 @@
   </si>
   <si>
     <t>1,5</t>
+  </si>
+  <si>
+    <t>Time in Hours</t>
+  </si>
+  <si>
+    <t>C = Time Completed</t>
+  </si>
+  <si>
+    <t>IP = Time Progressed thus far</t>
+  </si>
+  <si>
+    <t>IP</t>
   </si>
 </sst>
 </file>
@@ -75,7 +87,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -98,11 +110,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -122,6 +154,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37BCA52-A271-4118-AF0B-0601ADC60E68}">
-  <dimension ref="A1:Y6"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,131 +487,129 @@
     <col min="2" max="16384" width="3.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+    </row>
+    <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="3">
+      <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="3">
+      <c r="D2" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E2" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F2" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G2" s="3">
         <v>6</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H2" s="3">
         <v>7</v>
       </c>
-      <c r="I1" s="3">
+      <c r="I2" s="3">
         <v>8</v>
       </c>
-      <c r="J1" s="3">
+      <c r="J2" s="3">
         <v>9</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K2" s="3">
         <v>10</v>
       </c>
-      <c r="L1" s="3">
+      <c r="L2" s="3">
         <v>11</v>
       </c>
-      <c r="M1" s="3">
+      <c r="M2" s="3">
         <v>12</v>
       </c>
-      <c r="N1" s="3">
+      <c r="N2" s="3">
         <v>13</v>
       </c>
-      <c r="O1" s="3">
+      <c r="O2" s="3">
         <v>14</v>
       </c>
-      <c r="P1" s="3">
+      <c r="P2" s="3">
         <v>15</v>
       </c>
-      <c r="Q1" s="3">
+      <c r="Q2" s="3">
         <v>16</v>
       </c>
-      <c r="R1" s="3">
+      <c r="R2" s="3">
         <v>17</v>
       </c>
-      <c r="S1" s="3">
+      <c r="S2" s="3">
         <v>18</v>
       </c>
-      <c r="T1" s="3">
+      <c r="T2" s="3">
         <v>19</v>
       </c>
-      <c r="U1" s="3">
+      <c r="U2" s="3">
         <v>20</v>
       </c>
-      <c r="V1" s="3">
+      <c r="V2" s="3">
         <v>21</v>
       </c>
-      <c r="W1" s="3">
+      <c r="W2" s="3">
         <v>22</v>
       </c>
-      <c r="X1" s="3">
+      <c r="X2" s="3">
         <v>23</v>
       </c>
-      <c r="Y1" s="3">
+      <c r="Y2" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5">
-        <v>1</v>
-      </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
+        <v>0</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
       <c r="R3" s="4"/>
       <c r="S3" s="4"/>
@@ -585,12 +622,12 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="E4" s="6"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -598,15 +635,17 @@
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
@@ -616,7 +655,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -632,22 +671,22 @@
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="5">
-        <v>1</v>
-      </c>
+      <c r="P5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
       <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
-      <c r="W5" s="5"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
       <c r="X5" s="4"/>
       <c r="Y5" s="4"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -665,18 +704,63 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
       <c r="Q6" s="4"/>
-      <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="5" t="s">
+      <c r="R6" s="5">
+        <v>1</v>
+      </c>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="X6" s="5"/>
-      <c r="Y6" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:Y1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updatin Gantt Chart and Documentation
</commit_message>
<xml_diff>
--- a/doc/JAGanttChart.xlsx
+++ b/doc/JAGanttChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Programming\Team4Game\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C44040-4E80-4AD3-8DDA-9B3CD30F7CD3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7781D34-CEAD-4F26-874E-161039AE76EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="4440" xr2:uid="{6FA9B399-C385-4C01-A8E4-A4B4B0C49CEF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>1 Software Analysis</t>
   </si>
@@ -57,7 +57,13 @@
     <t>IP = Time Progressed thus far</t>
   </si>
   <si>
-    <t>IP</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Total Cost $2300</t>
+  </si>
+  <si>
+    <t>Estimated Cost $2400</t>
   </si>
 </sst>
 </file>
@@ -87,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -99,21 +105,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -130,37 +121,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37BCA52-A271-4118-AF0B-0601ADC60E68}">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,273 +536,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>4</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>6</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>7</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>8</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>9</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>10</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>11</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="2">
         <v>12</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="2">
         <v>13</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="2">
         <v>14</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="2">
         <v>15</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <v>16</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="2">
         <v>17</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="2">
         <v>18</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="2">
         <v>19</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2" s="2">
         <v>20</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="2">
         <v>21</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="2">
         <v>22</v>
       </c>
-      <c r="X2" s="3">
+      <c r="X2" s="2">
         <v>23</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Y2" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5">
+      <c r="E4" s="4"/>
+      <c r="M4" s="6">
         <v>1</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5" t="s">
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="5">
+      <c r="R6" s="6">
         <v>1</v>
       </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="3"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="5" t="s">
+      <c r="W7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
+      <c r="X7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="3"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Merge branch 'master' of https://github.com/atwo6777/Team4Game"
This reverts commit d7a34db0a86b16a3c0a99fa781d596f1f8f393e5, reversing
changes made to f09b794cda8a4acf6eec20f7154dd4bd102a3fa6.
</commit_message>
<xml_diff>
--- a/doc/JAGanttChart.xlsx
+++ b/doc/JAGanttChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Programming\Team4Game\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7781D34-CEAD-4F26-874E-161039AE76EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C44040-4E80-4AD3-8DDA-9B3CD30F7CD3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="4440" xr2:uid="{6FA9B399-C385-4C01-A8E4-A4B4B0C49CEF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>1 Software Analysis</t>
   </si>
@@ -57,13 +57,7 @@
     <t>IP = Time Progressed thus far</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Total Cost $2300</t>
-  </si>
-  <si>
-    <t>Estimated Cost $2400</t>
+    <t>IP</t>
   </si>
 </sst>
 </file>
@@ -93,12 +87,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -121,94 +130,37 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37BCA52-A271-4118-AF0B-0601ADC60E68}">
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,200 +488,273 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="3">
         <v>5</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="3">
         <v>6</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="3">
         <v>7</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="3">
         <v>8</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="3">
         <v>9</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="3">
         <v>10</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="3">
         <v>11</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="3">
         <v>12</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="3">
         <v>13</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="3">
         <v>14</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="3">
         <v>15</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="3">
         <v>16</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="3">
         <v>17</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="3">
         <v>18</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="3">
         <v>19</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="3">
         <v>20</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="3">
         <v>21</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="3">
         <v>22</v>
       </c>
-      <c r="X2" s="2">
+      <c r="X2" s="3">
         <v>23</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Y2" s="3">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="8" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="3"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+      <c r="U3" s="4"/>
+      <c r="V3" s="4"/>
+      <c r="W3" s="4"/>
+      <c r="X3" s="4"/>
+      <c r="Y3" s="4"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="M4" s="6">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="5">
         <v>1</v>
       </c>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7" t="s">
+      <c r="N4" s="5"/>
+      <c r="O4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="11"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+      <c r="U4" s="4"/>
+      <c r="V4" s="4"/>
+      <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="S5" s="3"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="4"/>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="R6" s="6">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
+      <c r="Q6" s="4"/>
+      <c r="R6" s="5">
         <v>1</v>
       </c>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="W6" s="3"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="W7" s="6" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="X7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="Y7" s="3"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/atwo6777/Team4Game""
This reverts commit 1231c14cf524d8a81b2b21c4afbe41238d647ed1.
</commit_message>
<xml_diff>
--- a/doc/JAGanttChart.xlsx
+++ b/doc/JAGanttChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Programming\Team4Game\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C44040-4E80-4AD3-8DDA-9B3CD30F7CD3}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7781D34-CEAD-4F26-874E-161039AE76EB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="4440" xr2:uid="{6FA9B399-C385-4C01-A8E4-A4B4B0C49CEF}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>1 Software Analysis</t>
   </si>
@@ -57,7 +57,13 @@
     <t>IP = Time Progressed thus far</t>
   </si>
   <si>
-    <t>IP</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Total Cost $2300</t>
+  </si>
+  <si>
+    <t>Estimated Cost $2400</t>
   </si>
 </sst>
 </file>
@@ -87,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -99,21 +105,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom style="thin">
@@ -130,37 +121,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37BCA52-A271-4118-AF0B-0601ADC60E68}">
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,273 +536,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
     </row>
     <row r="2" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>4</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>5</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>6</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>7</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>8</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2" s="2">
         <v>9</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="2">
         <v>10</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>11</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="2">
         <v>12</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="2">
         <v>13</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="2">
         <v>14</v>
       </c>
-      <c r="P2" s="3">
+      <c r="P2" s="2">
         <v>15</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="Q2" s="2">
         <v>16</v>
       </c>
-      <c r="R2" s="3">
+      <c r="R2" s="2">
         <v>17</v>
       </c>
-      <c r="S2" s="3">
+      <c r="S2" s="2">
         <v>18</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="2">
         <v>19</v>
       </c>
-      <c r="U2" s="3">
+      <c r="U2" s="2">
         <v>20</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="2">
         <v>21</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="2">
         <v>22</v>
       </c>
-      <c r="X2" s="3">
+      <c r="X2" s="2">
         <v>23</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="Y2" s="2">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
+      <c r="M3" s="3"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="5">
+      <c r="E4" s="4"/>
+      <c r="M4" s="6">
         <v>1</v>
       </c>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5" t="s">
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="4"/>
-      <c r="R4" s="4"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
+      <c r="Q4" s="11"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="5" t="s">
+      <c r="P5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="4"/>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
-      <c r="Y5" s="4"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="5">
+      <c r="R6" s="6">
         <v>1</v>
       </c>
-      <c r="S6" s="5"/>
-      <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="4"/>
-      <c r="Y6" s="4"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="3"/>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-      <c r="S7" s="4"/>
-      <c r="T7" s="4"/>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="5" t="s">
+      <c r="W7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="X7" s="5"/>
-      <c r="Y7" s="5"/>
+      <c r="X7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="3"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>